<commit_message>
working on inbevbr prod_seq
</commit_message>
<xml_diff>
--- a/Projects/CCBR_PROD/Data/Femsa template v4.5 - KENGINE.xlsx
+++ b/Projects/CCBR_PROD/Data/Femsa template v4.5 - KENGINE.xlsx
@@ -23,6 +23,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIS!$A$1:$E$126</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIS!$A$1:$E$126</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIS!$A$1:$E$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIS!$A$1:$E$126</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -891,7 +892,7 @@
     <t xml:space="preserve">GDM KOF CSD,GDM KOF NCB,GDM Proprio,GDM Conc</t>
   </si>
   <si>
-    <t xml:space="preserve">CSD FEMSA CC 1.5L REF PET,CSD FEMSA CC 2L REF PET,CSD FEMSA CC ZERO 2L REF PET,CSD FEMSA FT LAR 2L REF PET</t>
+    <t xml:space="preserve">CSD FEMSA CC 1.5L REF PET,CSD FEMSA CC 2L REF pet,CSD FEMSA CC ZERO 2L REF pet,CSD FEMSA FT LAR 2L REF pet</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;=</t>
@@ -2234,9 +2235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>393840</xdr:colOff>
+      <xdr:colOff>393480</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2246,7 +2247,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="18167400" cy="12730320"/>
+          <a:ext cx="17947800" cy="12729960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2276,9 +2277,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>393840</xdr:colOff>
+      <xdr:colOff>393480</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2288,7 +2289,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="18167400" cy="12730320"/>
+          <a:ext cx="17947800" cy="12729960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2318,9 +2319,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>113040</xdr:colOff>
+      <xdr:colOff>112680</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2330,7 +2331,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9418680" cy="9336600"/>
+          <a:ext cx="9313560" cy="9336240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2360,9 +2361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>113040</xdr:colOff>
+      <xdr:colOff>112680</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2372,7 +2373,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9418680" cy="9336600"/>
+          <a:ext cx="9313560" cy="9336240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2402,9 +2403,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9007920</xdr:colOff>
+      <xdr:colOff>9007560</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2414,7 +2415,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9007920" cy="9366480"/>
+          <a:ext cx="9007560" cy="9366120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2444,9 +2445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9007920</xdr:colOff>
+      <xdr:colOff>9007560</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2456,7 +2457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9007920" cy="9366480"/>
+          <a:ext cx="9007560" cy="9366120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2486,9 +2487,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2498,7 +2499,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9325440" cy="9367920"/>
+          <a:ext cx="9220320" cy="9367560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2528,9 +2529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2540,7 +2541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9325440" cy="9367920"/>
+          <a:ext cx="9220320" cy="9367560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2570,9 +2571,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>655200</xdr:colOff>
+      <xdr:colOff>654840</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2582,7 +2583,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9960840" cy="9442800"/>
+          <a:ext cx="9855720" cy="9442440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2612,9 +2613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>655200</xdr:colOff>
+      <xdr:colOff>654840</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2624,7 +2625,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9960840" cy="9442800"/>
+          <a:ext cx="9855720" cy="9442440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2655,18 +2656,18 @@
   </sheetPr>
   <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B52" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="116.632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="103"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="115.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4831,27 +4832,27 @@
   </sheetPr>
   <dimension ref="1:38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="148.760204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="124.05612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="111.908163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="11" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="13" style="11" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="75.1887755102041"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="103.673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="11" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="147.005102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="122.571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="110.55612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="52.9183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="11" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="13" style="11" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="74.2448979591837"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="102.591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="11" width="27.1326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18956,7 +18957,7 @@
       <c r="D27" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="18" t="s">
         <v>285</v>
       </c>
       <c r="F27" s="27"/>
@@ -23444,29 +23445,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="97.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="98.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="11" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="24" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="68.1683673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="70.8622448979592"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="11" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="11" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="35" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="168.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="11" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="96.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="97.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="11" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="24" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="67.3622448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="11" width="70.0612244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="11" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="11" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="11" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="35" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="11" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="166.581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="11" width="9.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -46397,12 +46398,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="131.887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="80.7244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="130.40306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>